<commit_message>
se establece maquetado del front
</commit_message>
<xml_diff>
--- a/backend/busqueda.xlsx
+++ b/backend/busqueda.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT\Documents\proyectos\api-scraping-ymk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT\Documents\proyectos\api-scraping-ymk\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -435,7 +435,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F11"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
se agrega funcionalidad de importar xlsx
</commit_message>
<xml_diff>
--- a/backend/busqueda.xlsx
+++ b/backend/busqueda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT\Documents\proyectos\api-scraping-ymk\backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\Proyectos_programación\api-scraping-ymk\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -435,7 +435,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A3" sqref="A3:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>